<commit_message>
change video gen and search
</commit_message>
<xml_diff>
--- a/data/question_answer/QA.xlsx
+++ b/data/question_answer/QA.xlsx
@@ -55,7 +55,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +66,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -102,17 +108,17 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -431,7 +437,7 @@
     <col min="4" max="4" style="6" width="38.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -445,7 +451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="44.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="46.5" customFormat="1" s="1">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -459,7 +465,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="44.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="46.5" customFormat="1" s="1">
       <c r="A3" s="4">
         <v>2</v>
       </c>

</xml_diff>